<commit_message>
Remove two wrong annotaions
</commit_message>
<xml_diff>
--- a/curator-annotations/strain-annotations/Strain Annotation-PMID-36524124-JAN-12-2023.xlsx
+++ b/curator-annotations/strain-annotations/Strain Annotation-PMID-36524124-JAN-12-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petrafey/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sba964/Projects/migration-data/curator-annotations/strain-annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35838720-B06A-9249-B0C1-6EF6C5A30CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524BF200-C692-914F-9E4C-1894921F4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1860" windowWidth="30060" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="600" windowWidth="25400" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strain_Annotations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Strain Descriptor</t>
   </si>
@@ -101,19 +101,13 @@
   </si>
   <si>
     <t>robert-dodson@northwestern.edu</t>
-  </si>
-  <si>
-    <t>This strain is in the Stock Center!!</t>
-  </si>
-  <si>
-    <t>please add that</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -127,13 +121,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -176,13 +163,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1344,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1462,9 +1448,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1482,9 +1466,7 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2041,41 +2023,41 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+    <row r="35" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
     </row>
     <row r="37" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
@@ -2203,42 +2185,6 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" xr:uid="{3EF3A7A5-46D2-8C42-A1D5-B676C619BDA3}"/>

</xml_diff>